<commit_message>
update DES for SED-BIOME with updated glossaries
</commit_message>
<xml_diff>
--- a/assets/projects/sed-biome/data-entry-spreadsheets/SED-BIOME_site-12_USA.xlsx
+++ b/assets/projects/sed-biome/data-entry-spreadsheets/SED-BIOME_site-12_USA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lonnemanm\Documents\repositories\marinegeo.github.io\assets\projects\sed-biome\data-entry-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FA3C33-7B82-4DB3-8408-6EB9F821C19D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7CDA96-60AA-44D1-9981-74A5B11E4EFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="28800" windowHeight="15555" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4065" yWindow="4065" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol_metadata" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="320">
   <si>
     <t>sheet</t>
   </si>
@@ -1117,6 +1117,15 @@
   <si>
     <t>fertilizer_presence_or_absence</t>
   </si>
+  <si>
+    <t>frame_fertilizer_presence</t>
+  </si>
+  <si>
+    <t>Indicate whether the sausages from the fertilised frames (with a red label) still contain fertilizer (presence) or not (absence).</t>
+  </si>
+  <si>
+    <t>presence; absence</t>
+  </si>
 </sst>
 </file>
 
@@ -1125,30 +1134,9 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="21">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1355,93 +1343,66 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1450,21 +1411,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -1472,28 +1427,56 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2089,7 +2072,7 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2108,7 +2091,7 @@
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2116,19 +2099,19 @@
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:2" ht="39.950000000000003" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="8"/>
     </row>
     <row r="5" spans="1:2" ht="39.950000000000003" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5" s="32">
         <v>12</v>
       </c>
     </row>
@@ -2136,73 +2119,73 @@
       <c r="A6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:2" ht="39.950000000000003" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="18"/>
     </row>
     <row r="8" spans="1:2" ht="39.950000000000003" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="24"/>
+      <c r="B8" s="18"/>
     </row>
     <row r="9" spans="1:2" ht="39.950000000000003" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="24"/>
+      <c r="B9" s="18"/>
     </row>
     <row r="10" spans="1:2" ht="39.950000000000003" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="8"/>
     </row>
     <row r="11" spans="1:2" ht="39.950000000000003" customHeight="1">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="23" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12:B1993 A10:B10 A3:B6 C1:Z1993">
-    <cfRule type="containsBlanks" dxfId="10" priority="9">
+    <cfRule type="containsBlanks" dxfId="14" priority="9">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsBlanks" dxfId="9" priority="7">
+    <cfRule type="containsBlanks" dxfId="13" priority="7">
       <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:B2">
-    <cfRule type="containsBlanks" dxfId="8" priority="6">
+    <cfRule type="containsBlanks" dxfId="12" priority="6">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="containsBlanks" dxfId="7" priority="5">
+    <cfRule type="containsBlanks" dxfId="11" priority="5">
       <formula>LEN(TRIM(A11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="containsBlanks" dxfId="6" priority="4">
+    <cfRule type="containsBlanks" dxfId="10" priority="4">
       <formula>LEN(TRIM(B11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:B9">
-    <cfRule type="containsBlanks" dxfId="5" priority="3">
+    <cfRule type="containsBlanks" dxfId="9" priority="3">
       <formula>LEN(TRIM(A7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="containsBlanks" dxfId="4" priority="1">
+    <cfRule type="containsBlanks" dxfId="8" priority="1">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2248,53 +2231,53 @@
     <col min="16" max="16" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="39" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:16" s="28" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A1" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="15" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2302,301 +2285,301 @@
       <c r="A2" s="1">
         <v>12</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="J2" s="11"/>
+      <c r="J2" s="10"/>
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="J3" s="11"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="J3" s="10"/>
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="J4" s="11"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="J4" s="10"/>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="J5" s="11"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="J5" s="10"/>
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="J6" s="11"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="J6" s="10"/>
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="J7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="J7" s="10"/>
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="J8" s="11"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="J8" s="10"/>
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="J9" s="11"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="J9" s="10"/>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="J10" s="11"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="J10" s="10"/>
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="J11" s="11"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="J11" s="10"/>
       <c r="M11" s="2"/>
     </row>
     <row r="12" spans="1:16">
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="J12" s="11"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="J12" s="10"/>
       <c r="M12" s="2"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="J13" s="11"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="J13" s="10"/>
       <c r="M13" s="2"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="J14" s="11"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="J14" s="10"/>
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="J15" s="11"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="J15" s="10"/>
       <c r="M15" s="2"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="J16" s="11"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="J16" s="10"/>
       <c r="M16" s="2"/>
     </row>
     <row r="17" spans="2:13">
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="J17" s="11"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="J17" s="10"/>
       <c r="M17" s="2"/>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="J18" s="11"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="J18" s="10"/>
       <c r="M18" s="2"/>
     </row>
     <row r="19" spans="2:13">
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="J19" s="11"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="J19" s="10"/>
       <c r="M19" s="2"/>
     </row>
     <row r="20" spans="2:13">
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="J20" s="11"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="J20" s="10"/>
       <c r="M20" s="2"/>
     </row>
     <row r="21" spans="2:13">
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="J21" s="11"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="J21" s="10"/>
       <c r="M21" s="2"/>
     </row>
     <row r="22" spans="2:13">
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="J22" s="11"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="J22" s="10"/>
       <c r="M22" s="2"/>
     </row>
     <row r="23" spans="2:13">
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="J23" s="11"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="J23" s="10"/>
       <c r="M23" s="2"/>
     </row>
     <row r="24" spans="2:13">
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="J24" s="11"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="J24" s="10"/>
       <c r="M24" s="2"/>
     </row>
     <row r="25" spans="2:13">
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="J25" s="11"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="J25" s="10"/>
       <c r="M25" s="2"/>
     </row>
     <row r="26" spans="2:13">
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="J26" s="11"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="J26" s="10"/>
       <c r="M26" s="2"/>
     </row>
     <row r="27" spans="2:13">
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="J27" s="11"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="J27" s="10"/>
       <c r="M27" s="2"/>
     </row>
     <row r="28" spans="2:13">
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="J28" s="11"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="J28" s="10"/>
       <c r="M28" s="2"/>
     </row>
     <row r="29" spans="2:13">
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="J29" s="11"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="J29" s="10"/>
       <c r="M29" s="2"/>
     </row>
     <row r="30" spans="2:13">
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="J30" s="11"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="J30" s="10"/>
       <c r="M30" s="2"/>
     </row>
     <row r="31" spans="2:13">
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="J31" s="11"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="J31" s="10"/>
       <c r="M31" s="2"/>
     </row>
     <row r="32" spans="2:13">
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="J32" s="11"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="J32" s="10"/>
       <c r="M32" s="2"/>
     </row>
     <row r="33" spans="2:13">
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="J33" s="11"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="J33" s="10"/>
       <c r="M33" s="2"/>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="J34" s="11"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="J34" s="10"/>
       <c r="M34" s="2"/>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="J35" s="11"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="J35" s="10"/>
       <c r="M35" s="2"/>
     </row>
     <row r="36" spans="2:13">
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="J36" s="11"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="J36" s="10"/>
       <c r="M36" s="2"/>
     </row>
     <row r="37" spans="2:13">
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="J37" s="11"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="J37" s="10"/>
       <c r="M37" s="2"/>
     </row>
     <row r="38" spans="2:13">
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="J38" s="11"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="J38" s="10"/>
       <c r="M38" s="2"/>
     </row>
     <row r="39" spans="2:13">
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="J39" s="11"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="J39" s="10"/>
       <c r="M39" s="2"/>
     </row>
     <row r="40" spans="2:13">
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="J40" s="11"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="J40" s="10"/>
       <c r="M40" s="2"/>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="J41" s="11"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="J41" s="10"/>
       <c r="M41" s="2"/>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="J42" s="11"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="J42" s="10"/>
       <c r="M42" s="2"/>
     </row>
     <row r="43" spans="2:13">
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="J43" s="11"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="J43" s="10"/>
       <c r="M43" s="2"/>
     </row>
     <row r="44" spans="2:13">
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="J44" s="11"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="J44" s="10"/>
       <c r="M44" s="2"/>
     </row>
     <row r="45" spans="2:13">
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="J45" s="11"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="J45" s="10"/>
       <c r="M45" s="2"/>
     </row>
     <row r="46" spans="2:13">
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="J46" s="11"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="J46" s="10"/>
       <c r="M46" s="2"/>
     </row>
     <row r="47" spans="2:13">
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="J47" s="11"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="J47" s="10"/>
       <c r="M47" s="2"/>
     </row>
     <row r="48" spans="2:13">
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="J48" s="11"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="J48" s="10"/>
       <c r="M48" s="2"/>
     </row>
     <row r="49" spans="2:13">
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="J49" s="11"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="J49" s="10"/>
       <c r="M49" s="2"/>
     </row>
     <row r="50" spans="2:13">
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="J50" s="11"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="J50" s="10"/>
       <c r="M50" s="2"/>
     </row>
   </sheetData>
@@ -2645,25 +2628,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2904,47 +2887,47 @@
     <col min="12" max="12" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="39" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:12" s="28" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="17" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="1">
         <v>12</v>
       </c>
@@ -2969,8 +2952,8 @@
       <c r="J2"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="1">
         <v>12</v>
       </c>
@@ -2995,8 +2978,8 @@
       <c r="J3"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="1">
         <v>12</v>
       </c>
@@ -3021,8 +3004,8 @@
       <c r="J4"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="1">
         <v>12</v>
       </c>
@@ -3047,8 +3030,8 @@
       <c r="J5"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="1">
         <v>12</v>
       </c>
@@ -3073,8 +3056,8 @@
       <c r="J6"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="1">
         <v>12</v>
       </c>
@@ -3099,8 +3082,8 @@
       <c r="J7"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="1">
         <v>12</v>
       </c>
@@ -3125,8 +3108,8 @@
       <c r="J8"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="1">
         <v>12</v>
       </c>
@@ -3151,8 +3134,8 @@
       <c r="J9"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="1">
         <v>12</v>
       </c>
@@ -3177,8 +3160,8 @@
       <c r="J10"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="1">
         <v>12</v>
       </c>
@@ -3203,8 +3186,8 @@
       <c r="J11"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="1">
         <v>12</v>
       </c>
@@ -3229,8 +3212,8 @@
       <c r="J12"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="1">
         <v>12</v>
       </c>
@@ -3255,8 +3238,8 @@
       <c r="J13"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="1">
         <v>12</v>
       </c>
@@ -3281,8 +3264,8 @@
       <c r="J14"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="1">
         <v>12</v>
       </c>
@@ -3307,8 +3290,8 @@
       <c r="J15"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="1">
         <v>12</v>
       </c>
@@ -3333,8 +3316,8 @@
       <c r="J16"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="1">
         <v>12</v>
       </c>
@@ -3359,8 +3342,8 @@
       <c r="J17"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="1">
         <v>12</v>
       </c>
@@ -3385,8 +3368,8 @@
       <c r="J18"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
       <c r="C19" s="1">
         <v>12</v>
       </c>
@@ -3411,8 +3394,8 @@
       <c r="J19"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
       <c r="C20" s="1">
         <v>12</v>
       </c>
@@ -3437,8 +3420,8 @@
       <c r="J20"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="1">
         <v>12</v>
       </c>
@@ -3463,8 +3446,8 @@
       <c r="J21"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="1">
         <v>12</v>
       </c>
@@ -3489,8 +3472,8 @@
       <c r="J22"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="1">
         <v>12</v>
       </c>
@@ -3515,8 +3498,8 @@
       <c r="J23"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="1">
         <v>12</v>
       </c>
@@ -3541,8 +3524,8 @@
       <c r="J24"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="1">
         <v>12</v>
       </c>
@@ -3567,8 +3550,8 @@
       <c r="J25"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="1">
         <v>12</v>
       </c>
@@ -3593,8 +3576,8 @@
       <c r="J26"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="1">
         <v>12</v>
       </c>
@@ -3619,8 +3602,8 @@
       <c r="J27"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="1">
         <v>12</v>
       </c>
@@ -3645,8 +3628,8 @@
       <c r="J28"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
       <c r="C29" s="1">
         <v>12</v>
       </c>
@@ -3671,8 +3654,8 @@
       <c r="J29"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
       <c r="C30" s="1">
         <v>12</v>
       </c>
@@ -3697,8 +3680,8 @@
       <c r="J30"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
       <c r="C31" s="1">
         <v>12</v>
       </c>
@@ -3723,8 +3706,8 @@
       <c r="J31"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
       <c r="C32" s="1">
         <v>12</v>
       </c>
@@ -3749,8 +3732,8 @@
       <c r="J32"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="1">
         <v>12</v>
       </c>
@@ -3775,8 +3758,8 @@
       <c r="J33"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
       <c r="C34" s="1">
         <v>12</v>
       </c>
@@ -3801,8 +3784,8 @@
       <c r="J34"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
       <c r="C35" s="1">
         <v>12</v>
       </c>
@@ -3827,8 +3810,8 @@
       <c r="J35"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
       <c r="C36" s="1">
         <v>12</v>
       </c>
@@ -3853,8 +3836,8 @@
       <c r="J36"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
       <c r="C37" s="1">
         <v>12</v>
       </c>
@@ -3879,8 +3862,8 @@
       <c r="J37"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
       <c r="C38" s="1">
         <v>12</v>
       </c>
@@ -3905,8 +3888,8 @@
       <c r="J38"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
       <c r="C39" s="1">
         <v>12</v>
       </c>
@@ -3931,8 +3914,8 @@
       <c r="J39"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="11"/>
-      <c r="B40" s="11"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
       <c r="C40" s="1">
         <v>12</v>
       </c>
@@ -3957,8 +3940,8 @@
       <c r="J40"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
       <c r="C41" s="1">
         <v>12</v>
       </c>
@@ -3983,8 +3966,8 @@
       <c r="J41"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
       <c r="C42" s="1">
         <v>12</v>
       </c>
@@ -4009,8 +3992,8 @@
       <c r="J42"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
       <c r="C43" s="1">
         <v>12</v>
       </c>
@@ -4035,8 +4018,8 @@
       <c r="J43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
       <c r="C44" s="1">
         <v>12</v>
       </c>
@@ -4061,8 +4044,8 @@
       <c r="J44"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="11"/>
-      <c r="B45" s="11"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
       <c r="C45" s="1">
         <v>12</v>
       </c>
@@ -4087,8 +4070,8 @@
       <c r="J45"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="11"/>
-      <c r="B46" s="11"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
       <c r="C46" s="1">
         <v>12</v>
       </c>
@@ -4113,8 +4096,8 @@
       <c r="J46"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
       <c r="C47" s="1">
         <v>12</v>
       </c>
@@ -4139,8 +4122,8 @@
       <c r="J47"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="11"/>
-      <c r="B48" s="11"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
       <c r="C48" s="1">
         <v>12</v>
       </c>
@@ -4165,8 +4148,8 @@
       <c r="J48"/>
     </row>
     <row r="49" spans="1:10">
-      <c r="A49" s="11"/>
-      <c r="B49" s="11"/>
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
       <c r="C49" s="1">
         <v>12</v>
       </c>
@@ -4191,8 +4174,8 @@
       <c r="J49"/>
     </row>
     <row r="50" spans="1:10">
-      <c r="A50" s="11"/>
-      <c r="B50" s="11"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
       <c r="C50" s="1">
         <v>12</v>
       </c>
@@ -4623,561 +4606,561 @@
     <col min="15" max="15" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="40" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:15" s="29" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="17" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="18">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="47">
-        <v>12</v>
-      </c>
-      <c r="E2" s="47">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="34">
+        <v>12</v>
+      </c>
+      <c r="E2" s="34">
         <v>1</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="35" t="s">
         <v>161</v>
       </c>
       <c r="K2">
         <f>I2*1000</f>
         <v>0</v>
       </c>
-      <c r="L2" s="34">
+      <c r="L2" s="25">
         <f>3.14*3.4*3.4</f>
         <v>36.298400000000001</v>
       </c>
-      <c r="M2" s="33" t="e">
+      <c r="M2" s="24" t="e">
         <f>K2/(L2*C3)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="47">
-        <v>12</v>
-      </c>
-      <c r="E3" s="47">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="34">
+        <v>12</v>
+      </c>
+      <c r="E3" s="34">
         <v>2</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="35" t="s">
         <v>162</v>
       </c>
       <c r="K3"/>
-      <c r="L3" s="34">
+      <c r="L3" s="25">
         <f t="shared" ref="L3:L7" si="0">3.14*3.4*3.4</f>
         <v>36.298400000000001</v>
       </c>
       <c r="M3"/>
     </row>
     <row r="4" spans="1:15" ht="15.75">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="47">
-        <v>12</v>
-      </c>
-      <c r="E4" s="47">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="34">
+        <v>12</v>
+      </c>
+      <c r="E4" s="34">
         <v>3</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="35" t="s">
         <v>163</v>
       </c>
       <c r="K4"/>
-      <c r="L4" s="34">
+      <c r="L4" s="25">
         <f t="shared" si="0"/>
         <v>36.298400000000001</v>
       </c>
       <c r="M4"/>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="47">
-        <v>12</v>
-      </c>
-      <c r="E5" s="47">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="34">
+        <v>12</v>
+      </c>
+      <c r="E5" s="34">
         <v>4</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="35" t="s">
         <v>164</v>
       </c>
       <c r="K5"/>
-      <c r="L5" s="34">
+      <c r="L5" s="25">
         <f t="shared" si="0"/>
         <v>36.298400000000001</v>
       </c>
       <c r="M5"/>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="47">
-        <v>12</v>
-      </c>
-      <c r="E6" s="47">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="34">
+        <v>12</v>
+      </c>
+      <c r="E6" s="34">
         <v>5</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="35" t="s">
         <v>165</v>
       </c>
       <c r="K6"/>
-      <c r="L6" s="34">
+      <c r="L6" s="25">
         <f t="shared" si="0"/>
         <v>36.298400000000001</v>
       </c>
       <c r="M6"/>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="47">
-        <v>12</v>
-      </c>
-      <c r="E7" s="47">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="34">
+        <v>12</v>
+      </c>
+      <c r="E7" s="34">
         <v>6</v>
       </c>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="35" t="s">
         <v>166</v>
       </c>
       <c r="K7"/>
-      <c r="L7" s="34">
+      <c r="L7" s="25">
         <f t="shared" si="0"/>
         <v>36.298400000000001</v>
       </c>
       <c r="M7"/>
     </row>
     <row r="8" spans="1:15" ht="18">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
       <c r="F8"/>
       <c r="K8"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
       <c r="F9"/>
       <c r="K9"/>
       <c r="L9"/>
       <c r="M9"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
       <c r="F10"/>
       <c r="K10"/>
       <c r="L10"/>
       <c r="M10"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
       <c r="F11"/>
       <c r="K11"/>
       <c r="L11"/>
       <c r="M11"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
       <c r="F12"/>
       <c r="K12"/>
       <c r="L12"/>
       <c r="M12"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
       <c r="F13"/>
       <c r="K13"/>
       <c r="L13"/>
       <c r="M13"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
       <c r="F14"/>
       <c r="K14"/>
       <c r="L14"/>
       <c r="M14"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
       <c r="F15"/>
       <c r="K15"/>
       <c r="L15"/>
       <c r="M15"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
       <c r="F16"/>
       <c r="K16"/>
       <c r="L16"/>
       <c r="M16"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
       <c r="F17"/>
       <c r="K17"/>
       <c r="L17"/>
       <c r="M17"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
       <c r="F18"/>
       <c r="K18"/>
       <c r="L18"/>
       <c r="M18"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
       <c r="F19"/>
       <c r="K19"/>
       <c r="L19"/>
       <c r="M19"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
       <c r="F20"/>
       <c r="K20"/>
       <c r="L20"/>
       <c r="M20"/>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
       <c r="F21"/>
       <c r="K21"/>
       <c r="L21"/>
       <c r="M21"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
       <c r="F22"/>
       <c r="K22"/>
       <c r="L22"/>
       <c r="M22"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
       <c r="F23"/>
       <c r="K23"/>
       <c r="L23"/>
       <c r="M23"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
       <c r="F24"/>
       <c r="K24"/>
       <c r="L24"/>
       <c r="M24"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
       <c r="F25"/>
       <c r="K25"/>
       <c r="L25"/>
       <c r="M25"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
       <c r="F26"/>
       <c r="K26"/>
       <c r="L26"/>
       <c r="M26"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
       <c r="F27"/>
       <c r="K27"/>
       <c r="L27"/>
       <c r="M27"/>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
       <c r="F28"/>
       <c r="K28"/>
       <c r="L28"/>
       <c r="M28"/>
     </row>
     <row r="29" spans="1:13">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
       <c r="F29"/>
       <c r="K29"/>
       <c r="L29"/>
       <c r="M29"/>
     </row>
     <row r="30" spans="1:13">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
       <c r="F30"/>
       <c r="K30"/>
       <c r="L30"/>
       <c r="M30"/>
     </row>
     <row r="31" spans="1:13">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
       <c r="F31"/>
       <c r="K31"/>
       <c r="L31"/>
       <c r="M31"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
       <c r="F32"/>
       <c r="K32"/>
       <c r="L32"/>
       <c r="M32"/>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
       <c r="F33"/>
       <c r="K33"/>
       <c r="L33"/>
       <c r="M33"/>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
       <c r="F34"/>
       <c r="K34"/>
       <c r="L34"/>
       <c r="M34"/>
     </row>
     <row r="35" spans="1:13">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
       <c r="F35"/>
       <c r="K35"/>
       <c r="L35"/>
       <c r="M35"/>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
       <c r="F36"/>
       <c r="K36"/>
       <c r="L36"/>
       <c r="M36"/>
     </row>
     <row r="37" spans="1:13">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
       <c r="F37"/>
       <c r="K37"/>
       <c r="L37"/>
       <c r="M37"/>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
       <c r="F38"/>
       <c r="K38"/>
       <c r="L38"/>
       <c r="M38"/>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
       <c r="F39"/>
       <c r="K39"/>
       <c r="L39"/>
       <c r="M39"/>
     </row>
     <row r="40" spans="1:13">
-      <c r="A40" s="11"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
       <c r="F40"/>
       <c r="K40"/>
       <c r="L40"/>
       <c r="M40"/>
     </row>
     <row r="41" spans="1:13">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
       <c r="F41"/>
       <c r="K41"/>
       <c r="L41"/>
       <c r="M41"/>
     </row>
     <row r="42" spans="1:13">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
       <c r="F42"/>
       <c r="K42"/>
       <c r="L42"/>
       <c r="M42"/>
     </row>
     <row r="43" spans="1:13">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
       <c r="F43"/>
       <c r="K43"/>
       <c r="L43"/>
       <c r="M43"/>
     </row>
     <row r="44" spans="1:13">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
       <c r="F44"/>
       <c r="K44"/>
       <c r="L44"/>
       <c r="M44"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="11"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
       <c r="F45"/>
       <c r="K45"/>
       <c r="L45"/>
       <c r="M45"/>
     </row>
     <row r="46" spans="1:13">
-      <c r="A46" s="11"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
       <c r="F46"/>
       <c r="K46"/>
       <c r="L46"/>
       <c r="M46"/>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
       <c r="F47"/>
       <c r="K47"/>
       <c r="L47"/>
       <c r="M47"/>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="11"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
       <c r="F48"/>
       <c r="K48"/>
       <c r="L48"/>
       <c r="M48"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" s="11"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
       <c r="F49"/>
       <c r="K49"/>
       <c r="L49"/>
       <c r="M49"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" s="11"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
       <c r="F50"/>
       <c r="K50"/>
       <c r="L50"/>
@@ -5305,7 +5288,7 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -5318,20 +5301,20 @@
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="40" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:5" s="29" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A1" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="17" t="s">
         <v>51</v>
       </c>
     </row>
@@ -5400,7 +5383,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="23" type="noConversion"/>
+  <phoneticPr fontId="20" type="noConversion"/>
   <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Weight, in grams of the tea bags. Please refer to the protocol for instructions for weighing the tea bags." sqref="C1" xr:uid="{E1259F66-B169-49EA-AB68-E145AD8A044E}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any additional notes regarding observations, context, or concerns about the data." sqref="E1" xr:uid="{14337A96-194D-4BB0-ADE0-653DD6AFF133}"/>
@@ -5418,23 +5401,23 @@
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="50.1" customHeight="1"/>
   <cols>
-    <col min="1" max="3" width="40.7109375" style="20" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" style="20" customWidth="1"/>
-    <col min="6" max="7" width="18.7109375" style="20" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="20"/>
+    <col min="1" max="3" width="40.7109375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="22" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" style="22" customWidth="1"/>
+    <col min="6" max="7" width="18.7109375" style="22" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="18" customFormat="1" ht="15.75">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5454,19 +5437,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="14" customFormat="1" ht="56.1" customHeight="1">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:6" s="12" customFormat="1" ht="56.1" customHeight="1">
+      <c r="A2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:6" s="18" customFormat="1" ht="56.1" customHeight="1">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:6" ht="56.1" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>36</v>
       </c>
@@ -5482,7 +5465,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" s="18" customFormat="1" ht="56.1" customHeight="1">
+    <row r="4" spans="1:6" ht="56.1" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>36</v>
       </c>
@@ -5498,7 +5481,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" s="18" customFormat="1" ht="56.1" customHeight="1">
+    <row r="5" spans="1:6" ht="56.1" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>36</v>
       </c>
@@ -5514,7 +5497,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" s="18" customFormat="1" ht="100.5" customHeight="1">
+    <row r="6" spans="1:6" ht="100.5" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>36</v>
       </c>
@@ -5530,7 +5513,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" s="18" customFormat="1" ht="56.1" customHeight="1">
+    <row r="7" spans="1:6" ht="56.1" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>36</v>
       </c>
@@ -5548,7 +5531,7 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" s="18" customFormat="1" ht="56.1" customHeight="1">
+    <row r="8" spans="1:6" ht="56.1" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>36</v>
       </c>
@@ -5566,7 +5549,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" s="18" customFormat="1" ht="76.5" customHeight="1">
+    <row r="9" spans="1:6" ht="76.5" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>36</v>
       </c>
@@ -5584,7 +5567,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" s="18" customFormat="1" ht="56.1" customHeight="1">
+    <row r="10" spans="1:6" ht="56.1" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>36</v>
       </c>
@@ -5600,7 +5583,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" s="14" customFormat="1" ht="56.1" customHeight="1">
+    <row r="11" spans="1:6" s="12" customFormat="1" ht="56.1" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>36</v>
       </c>
@@ -5618,7 +5601,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" s="18" customFormat="1" ht="56.1" customHeight="1">
+    <row r="12" spans="1:6" ht="56.1" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>36</v>
       </c>
@@ -5634,19 +5617,19 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" s="18" customFormat="1" ht="56.1" customHeight="1">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:6" ht="56.1" customHeight="1">
+      <c r="A13" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:6" s="18" customFormat="1" ht="105.75" customHeight="1">
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:6" ht="105.75" customHeight="1">
       <c r="A14" s="7" t="s">
         <v>136</v>
       </c>
@@ -5662,7 +5645,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" s="31" customFormat="1" ht="76.5" customHeight="1">
+    <row r="15" spans="1:6" ht="76.5" customHeight="1">
       <c r="A15" s="7" t="s">
         <v>136</v>
       </c>
@@ -5674,7 +5657,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" s="31" customFormat="1" ht="76.5" customHeight="1">
+    <row r="16" spans="1:6" ht="76.5" customHeight="1">
       <c r="A16" s="7" t="s">
         <v>136</v>
       </c>
@@ -5686,7 +5669,7 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6" s="18" customFormat="1" ht="49.5" customHeight="1">
+    <row r="17" spans="1:6" ht="49.5" customHeight="1">
       <c r="A17" s="7" t="s">
         <v>136</v>
       </c>
@@ -5704,7 +5687,7 @@
       </c>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" s="14" customFormat="1" ht="56.1" customHeight="1">
+    <row r="18" spans="1:6" s="12" customFormat="1" ht="56.1" customHeight="1">
       <c r="A18" s="7" t="s">
         <v>136</v>
       </c>
@@ -5722,7 +5705,7 @@
       </c>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" s="14" customFormat="1" ht="56.1" customHeight="1">
+    <row r="19" spans="1:6" s="12" customFormat="1" ht="56.1" customHeight="1">
       <c r="A19" s="7" t="s">
         <v>136</v>
       </c>
@@ -5740,7 +5723,7 @@
       </c>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:6" s="18" customFormat="1" ht="56.1" customHeight="1">
+    <row r="20" spans="1:6" ht="56.1" customHeight="1">
       <c r="A20" s="7" t="s">
         <v>136</v>
       </c>
@@ -5758,11 +5741,11 @@
       </c>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="1:6" s="28" customFormat="1" ht="60" customHeight="1">
+    <row r="21" spans="1:6" ht="60" customHeight="1">
       <c r="A21" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="14" t="s">
         <v>140</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -5776,11 +5759,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="28" customFormat="1" ht="60" customHeight="1">
+    <row r="22" spans="1:6" ht="60" customHeight="1">
       <c r="A22" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="14" t="s">
         <v>141</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -5794,7 +5777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="31" customFormat="1" ht="62.25" customHeight="1">
+    <row r="23" spans="1:6" ht="62.25" customHeight="1">
       <c r="A23" s="7" t="s">
         <v>136</v>
       </c>
@@ -5808,7 +5791,7 @@
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:6" s="28" customFormat="1" ht="60" customHeight="1">
+    <row r="24" spans="1:6" ht="60" customHeight="1">
       <c r="A24" s="7" t="s">
         <v>136</v>
       </c>
@@ -5824,7 +5807,7 @@
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:6" s="18" customFormat="1" ht="59.25" customHeight="1">
+    <row r="25" spans="1:6" ht="59.25" customHeight="1">
       <c r="A25" s="7" t="s">
         <v>136</v>
       </c>
@@ -5838,7 +5821,7 @@
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:6" s="18" customFormat="1" ht="48" customHeight="1">
+    <row r="26" spans="1:6" ht="48" customHeight="1">
       <c r="A26" s="7" t="s">
         <v>136</v>
       </c>
@@ -5856,11 +5839,11 @@
       </c>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="1:6" s="18" customFormat="1" ht="63" customHeight="1">
+    <row r="27" spans="1:6" ht="63" customHeight="1">
       <c r="A27" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="19" t="s">
         <v>53</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -5872,11 +5855,11 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:6" s="18" customFormat="1" ht="78.75" customHeight="1">
+    <row r="28" spans="1:6" ht="78.75" customHeight="1">
       <c r="A28" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -5888,11 +5871,11 @@
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:6" s="18" customFormat="1" ht="53.1" customHeight="1">
+    <row r="29" spans="1:6" ht="53.1" customHeight="1">
       <c r="A29" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="19" t="s">
         <v>50</v>
       </c>
       <c r="C29" s="7" t="s">
@@ -5904,347 +5887,347 @@
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" s="18" customFormat="1" ht="47.1" customHeight="1">
-      <c r="A30" s="12" t="s">
+    <row r="30" spans="1:6" ht="47.1" customHeight="1">
+      <c r="A30" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12" t="s">
+      <c r="B30" s="11"/>
+      <c r="C30" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="1:6" s="18" customFormat="1" ht="51" customHeight="1">
-      <c r="A31" s="41" t="s">
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="1:6" ht="90.75" customHeight="1">
+      <c r="A31" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="41" t="s">
+      <c r="D31" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-    </row>
-    <row r="32" spans="1:6" s="18" customFormat="1" ht="51" customHeight="1">
-      <c r="A32" s="41" t="s">
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+    </row>
+    <row r="32" spans="1:6" ht="51" customHeight="1">
+      <c r="A32" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="C32" s="41" t="s">
+      <c r="C32" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-    </row>
-    <row r="33" spans="1:6" s="18" customFormat="1" ht="51" customHeight="1">
-      <c r="A33" s="41" t="s">
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+    </row>
+    <row r="33" spans="1:6" ht="51" customHeight="1">
+      <c r="A33" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="D33" s="41" t="s">
+      <c r="D33" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-    </row>
-    <row r="34" spans="1:6" s="18" customFormat="1" ht="51" customHeight="1">
-      <c r="A34" s="41" t="s">
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+    </row>
+    <row r="34" spans="1:6" ht="51" customHeight="1">
+      <c r="A34" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-    </row>
-    <row r="35" spans="1:6" s="18" customFormat="1" ht="51" customHeight="1">
-      <c r="A35" s="41" t="s">
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+    </row>
+    <row r="35" spans="1:6" ht="51" customHeight="1">
+      <c r="A35" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="41" t="s">
+      <c r="C35" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="41" t="s">
+      <c r="D35" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-    </row>
-    <row r="36" spans="1:6" s="18" customFormat="1" ht="51" customHeight="1">
-      <c r="A36" s="41" t="s">
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+    </row>
+    <row r="36" spans="1:6" ht="51" customHeight="1">
+      <c r="A36" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="C36" s="41" t="s">
+      <c r="C36" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="41" t="s">
+      <c r="D36" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-    </row>
-    <row r="37" spans="1:6" s="18" customFormat="1" ht="51" customHeight="1">
-      <c r="A37" s="41" t="s">
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+    </row>
+    <row r="37" spans="1:6" ht="51" customHeight="1">
+      <c r="A37" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="41" t="s">
+      <c r="D37" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-    </row>
-    <row r="38" spans="1:6" s="18" customFormat="1" ht="51" customHeight="1">
-      <c r="A38" s="12" t="s">
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+    </row>
+    <row r="38" spans="1:6" ht="51" customHeight="1">
+      <c r="A38" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12" t="s">
+      <c r="B38" s="11"/>
+      <c r="C38" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-    </row>
-    <row r="39" spans="1:6" s="35" customFormat="1" ht="56.1" customHeight="1">
-      <c r="A39" s="10" t="s">
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+    </row>
+    <row r="39" spans="1:6" ht="56.1" customHeight="1">
+      <c r="A39" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D39" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E39" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F39" s="17"/>
+      <c r="F39" s="21"/>
     </row>
     <row r="40" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="30" t="s">
+      <c r="C40" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="D40" s="30" t="s">
+      <c r="D40" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E40" s="30" t="s">
+      <c r="E40" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="30"/>
-    </row>
-    <row r="41" spans="1:6" s="15" customFormat="1" ht="52.5" customHeight="1">
-      <c r="A41" s="10" t="s">
+      <c r="F40" s="21"/>
+    </row>
+    <row r="41" spans="1:6" s="37" customFormat="1" ht="103.5" customHeight="1">
+      <c r="A41" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C41" s="30" t="s">
+      <c r="C41" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D41" s="30" t="s">
+      <c r="D41" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-    </row>
-    <row r="42" spans="1:6" s="15" customFormat="1" ht="52.5" customHeight="1">
-      <c r="A42" s="10" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+    </row>
+    <row r="42" spans="1:6" s="37" customFormat="1" ht="52.5" customHeight="1">
+      <c r="A42" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D42" s="30" t="s">
+      <c r="D42" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-    </row>
-    <row r="43" spans="1:6" s="28" customFormat="1" ht="54" customHeight="1">
-      <c r="A43" s="10" t="s">
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+    </row>
+    <row r="43" spans="1:6" ht="54" customHeight="1">
+      <c r="A43" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="D43" s="30" t="s">
+      <c r="D43" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-    </row>
-    <row r="44" spans="1:6" s="15" customFormat="1" ht="52.5" customHeight="1">
-      <c r="A44" s="10" t="s">
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+    </row>
+    <row r="44" spans="1:6" s="37" customFormat="1" ht="52.5" customHeight="1">
+      <c r="A44" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B44" s="29" t="s">
+      <c r="B44" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="30" t="s">
+      <c r="C44" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D44" s="30" t="s">
+      <c r="D44" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
     </row>
     <row r="45" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C45" s="30" t="s">
+      <c r="C45" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="D45" s="30" t="s">
+      <c r="D45" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
     </row>
     <row r="46" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C46" s="30" t="s">
+      <c r="C46" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
     </row>
     <row r="47" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C47" s="30" t="s">
+      <c r="C47" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D47" s="27" t="s">
+      <c r="D47" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
     </row>
     <row r="48" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C48" s="30" t="s">
+      <c r="C48" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="D48" s="27" t="s">
+      <c r="D48" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E48" s="30" t="s">
+      <c r="E48" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="F48" s="30" t="s">
+      <c r="F48" s="21" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="29" t="s">
+      <c r="B49" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C49" s="29" t="s">
+      <c r="C49" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D49" s="29" t="s">
+      <c r="D49" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
     </row>
     <row r="50" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="C50" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D50" s="17" t="s">
+      <c r="D50" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
     </row>
     <row r="51" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12" t="s">
+      <c r="B51" s="11"/>
+      <c r="C51" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
     </row>
     <row r="52" spans="1:6" ht="50.1" customHeight="1">
       <c r="A52" s="6" t="s">
@@ -6298,7 +6281,7 @@
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" spans="1:6" ht="50.1" customHeight="1">
+    <row r="55" spans="1:6" ht="85.5" customHeight="1">
       <c r="A55" s="6" t="s">
         <v>117</v>
       </c>
@@ -6334,7 +6317,7 @@
       <c r="A57" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B57" s="44" t="s">
+      <c r="B57" s="31" t="s">
         <v>92</v>
       </c>
       <c r="C57" s="6" t="s">
@@ -6390,7 +6373,7 @@
       <c r="A60" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B60" s="37" t="s">
+      <c r="B60" s="31" t="s">
         <v>95</v>
       </c>
       <c r="C60" s="6" t="s">
@@ -6410,7 +6393,7 @@
       <c r="A61" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B61" s="38" t="s">
+      <c r="B61" s="27" t="s">
         <v>96</v>
       </c>
       <c r="C61" s="6" t="s">
@@ -6426,7 +6409,7 @@
       <c r="A62" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="38" t="s">
+      <c r="B62" s="27" t="s">
         <v>97</v>
       </c>
       <c r="C62" s="6" t="s">
@@ -6446,7 +6429,7 @@
       <c r="A63" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B63" s="38" t="s">
+      <c r="B63" s="27" t="s">
         <v>98</v>
       </c>
       <c r="C63" s="6" t="s">
@@ -6466,7 +6449,7 @@
       <c r="A64" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B64" s="38" t="s">
+      <c r="B64" s="27" t="s">
         <v>99</v>
       </c>
       <c r="C64" s="6" t="s">
@@ -6513,147 +6496,241 @@
       <c r="F66" s="6"/>
     </row>
     <row r="67" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A67" s="12" t="s">
+      <c r="A67" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="B67" s="11"/>
+      <c r="C67" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+    </row>
+    <row r="68" spans="1:6" ht="84" customHeight="1">
+      <c r="A68" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C68" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D68" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
+    </row>
+    <row r="69" spans="1:6" ht="50.1" customHeight="1">
+      <c r="A69" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="B69" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C69" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D69" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+    </row>
+    <row r="70" spans="1:6" ht="67.5" customHeight="1">
+      <c r="A70" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="B70" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="C70" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="D70" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" s="21" t="s">
+        <v>319</v>
+      </c>
+      <c r="F70" s="21"/>
+    </row>
+    <row r="71" spans="1:6" ht="50.1" customHeight="1">
+      <c r="A71" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="B71" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C71" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D71" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
+    </row>
+    <row r="72" spans="1:6" ht="50.1" customHeight="1">
+      <c r="A72" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="B72" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C72" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D72" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+    </row>
+    <row r="73" spans="1:6" ht="50.1" customHeight="1">
+      <c r="A73" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12" t="s">
+      <c r="B73" s="11"/>
+      <c r="C73" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D67" s="12"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="12"/>
-    </row>
-    <row r="68" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A68" s="7" t="s">
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+    </row>
+    <row r="74" spans="1:6" ht="50.1" customHeight="1">
+      <c r="A74" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B74" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C74" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D74" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E68" s="8"/>
-      <c r="F68" s="7"/>
-    </row>
-    <row r="69" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A69" s="7" t="s">
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+    </row>
+    <row r="75" spans="1:6" ht="50.1" customHeight="1">
+      <c r="A75" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B75" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C75" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D75" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E69" s="8"/>
-      <c r="F69" s="8"/>
-    </row>
-    <row r="70" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A70" s="7" t="s">
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+    </row>
+    <row r="76" spans="1:6" ht="50.1" customHeight="1">
+      <c r="A76" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B76" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C70" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D70" s="7" t="s">
+      <c r="C76" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E70" s="8"/>
-      <c r="F70" s="8"/>
-    </row>
-    <row r="71" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A71" s="7" t="s">
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+    </row>
+    <row r="77" spans="1:6" ht="50.1" customHeight="1">
+      <c r="A77" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B77" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="C77" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="D77" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E71" s="8"/>
-      <c r="F71" s="8"/>
-    </row>
-    <row r="72" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A72" s="7" t="s">
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+    </row>
+    <row r="78" spans="1:6" ht="50.1" customHeight="1">
+      <c r="A78" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B78" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="C78" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D78" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E72" s="8"/>
-      <c r="F72" s="7"/>
-    </row>
-    <row r="73" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A73" s="7" t="s">
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+    </row>
+    <row r="79" spans="1:6" ht="50.1" customHeight="1">
+      <c r="A79" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="B79" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C73" s="7" t="s">
+      <c r="C79" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D73" s="7" t="s">
+      <c r="D79" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E73" s="8"/>
-      <c r="F73" s="8"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:B5 B10:B12">
-    <cfRule type="containsBlanks" dxfId="3" priority="5">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="containsBlanks" dxfId="2" priority="4">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="containsBlanks" dxfId="1" priority="3">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="containsBlanks" dxfId="0" priority="2">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(B7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="12">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The sheet in which the field occurs" sqref="A1" xr:uid="{00000000-0002-0000-0400-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the field being defined" sqref="B1" xr:uid="{00000000-0002-0000-0400-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The field definition" sqref="C1" xr:uid="{00000000-0002-0000-0400-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The type of entry that should occupy the field (e.g., text, decimal, integer, date, etc…)" sqref="D1" xr:uid="{00000000-0002-0000-0400-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The format the field should follow" sqref="E1" xr:uid="{00000000-0002-0000-0400-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The units the field should contain" sqref="F1" xr:uid="{00000000-0002-0000-0400-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="B17:B26" xr:uid="{00000000-0002-0000-0400-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The frame at the location the sample came from: 1:16" sqref="B57" xr:uid="{C3FBA85C-CD9B-4BD6-A1F6-DC5A974F2955}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique number of the sampled tea bag (1-64)." sqref="B60" xr:uid="{71709EE2-7347-4053-8297-B2F55B2BF556}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of data collector(s)" sqref="B35" xr:uid="{95A169F1-633F-4E38-8BCE-BB264F757CA0}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="B32:B34" xr:uid="{291C9273-1D57-4BFC-A76B-3F61669EA188}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Full name of the data entry person" sqref="B36" xr:uid="{FF46A50E-051A-43DD-9EA8-0CD1E0632004}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The sheet in which the field occurs" sqref="A1" xr:uid="{02491648-BC7D-48AF-8F21-478A5AF148BA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the field being defined" sqref="B1" xr:uid="{A49E4808-BB3A-485B-9854-4557A91F8C23}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The field definition" sqref="C1" xr:uid="{7A167ACE-4FEF-4C8A-A147-D2F2D950EE16}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The type of entry that should occupy the field (e.g., text, decimal, integer, date, etc…)" sqref="D1" xr:uid="{6711C5BC-65DD-4CDD-BAEC-E2C166336743}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The format the field should follow" sqref="E1" xr:uid="{7E85A1AF-9C53-4649-B7D0-CE125D79C1F0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The units the field should contain" sqref="F1" xr:uid="{34271EA6-E22C-43F0-9EFA-637739CFE419}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="B17:B26" xr:uid="{DB3472B7-886F-41B4-A3E5-1B8074A95A26}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The frame at the location the sample came from: 1:16" sqref="B57" xr:uid="{AD31378E-0943-4B7F-B2D6-953C0791F8E0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique number of the sampled tea bag (1-64)." sqref="B60" xr:uid="{A058C8DC-AF90-401A-84EB-9775AC16FB02}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of data collector(s)" sqref="B35" xr:uid="{E8634BA1-B08F-4CA4-8583-384F28A62A37}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="B32:B34" xr:uid="{96D980AB-7A72-40D8-A8CE-E26CDA72EF90}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Full name of the data entry person" sqref="B36" xr:uid="{988B11FE-9EF2-4956-8567-640E029C84A2}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>